<commit_message>
added cap part sources
</commit_message>
<xml_diff>
--- a/Hardware/Motherboard_BOM.xlsx
+++ b/Hardware/Motherboard_BOM.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Motherboard!$A$1:$D$221</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="319">
   <si>
     <t>Part</t>
   </si>
@@ -902,13 +905,82 @@
   </si>
   <si>
     <t>Y5</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Quant</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12061a220jat2a/capacitor-ceramic-22pf-100v-c0g/dp/96K4783</t>
+  </si>
+  <si>
+    <t>96K4783</t>
+  </si>
+  <si>
+    <t>96M1466</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12061c104jat2a/capacitor-ceramic-0-1uf-100v-x7r/dp/96M1466</t>
+  </si>
+  <si>
+    <t>30H0930</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12061a222jat2a/capacitor-ceramic-2200pf-100v/dp/30H0930</t>
+  </si>
+  <si>
+    <t>96M1464</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12061c103jat2a/capacitor-ceramic-0-01uf-100v/dp/96M1464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94W2957 </t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12065a180jat2a/capacitor-ceramic-18pf-50v-c0g/dp/94W2957</t>
+  </si>
+  <si>
+    <t>20pF</t>
+  </si>
+  <si>
+    <t>70K9303</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/kemet/c1206c200j5gactu/capacitor-ceramic-20pf-50v-c0g/dp/70K9303</t>
+  </si>
+  <si>
+    <t>2200pF</t>
+  </si>
+  <si>
+    <t>60R6374</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12063d106kat2a/capacitor-ceramic-10uf-25v-x5r/dp/60R6374</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96K4787 </t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12063c105kat2a/capacitor-ceramic-1uf-25v-x7r/dp/96K4787</t>
+  </si>
+  <si>
+    <t>10nF/0.01uF</t>
+  </si>
+  <si>
+    <t>60R6372</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1044,8 +1116,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1225,6 +1305,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1342,7 +1428,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1385,11 +1471,19 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1423,6 +1517,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1730,3098 +1825,3239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D221"/>
+  <dimension ref="A1:I221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="84.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="H3" s="1">
+        <v>56</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F5" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>1206</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1206</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>1206</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1206</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="F10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19">
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21">
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28">
+      <c r="C28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29">
+      <c r="C29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36">
+      <c r="C36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39">
+      <c r="C39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40">
+      <c r="C40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41">
+      <c r="C41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42">
+      <c r="C42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43">
+      <c r="C43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44">
+      <c r="C44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45">
+      <c r="C45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C46" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46">
+      <c r="C46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C47" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47">
+      <c r="C47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C48" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48">
+      <c r="C48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C49" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49">
+      <c r="C49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D50">
+      <c r="C50" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C51" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51">
+      <c r="C51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C52" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52">
+      <c r="C52" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C53" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53">
+      <c r="C53" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C54" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54">
+      <c r="C54" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C55" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55">
+      <c r="C55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C56" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56">
+      <c r="C56" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57">
+      <c r="C57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C58" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58">
+      <c r="C58" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C59" t="s">
-        <v>18</v>
-      </c>
-      <c r="D59">
+      <c r="C59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C60" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60">
+      <c r="C60" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C61" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61">
+      <c r="C61" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C62" t="s">
-        <v>18</v>
-      </c>
-      <c r="D62">
+      <c r="C62" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C63" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63">
+      <c r="C63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C64" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64">
+      <c r="C64" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D65">
+      <c r="C65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D65" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C66" t="s">
-        <v>18</v>
-      </c>
-      <c r="D66">
+      <c r="C66" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C67" t="s">
-        <v>18</v>
-      </c>
-      <c r="D67">
+      <c r="C67" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C68" t="s">
-        <v>18</v>
-      </c>
-      <c r="D68">
+      <c r="C68" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C69" t="s">
-        <v>18</v>
-      </c>
-      <c r="D69">
+      <c r="C69" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C70" t="s">
-        <v>18</v>
-      </c>
-      <c r="D70">
+      <c r="C70" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C71" t="s">
-        <v>18</v>
-      </c>
-      <c r="D71">
+      <c r="C71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C72" t="s">
-        <v>18</v>
-      </c>
-      <c r="D72">
+      <c r="C72" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C73" t="s">
-        <v>18</v>
-      </c>
-      <c r="D73">
+      <c r="C73" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C74" t="s">
-        <v>18</v>
-      </c>
-      <c r="D74">
+      <c r="C74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C75" t="s">
-        <v>18</v>
-      </c>
-      <c r="D75">
+      <c r="C75" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C76" t="s">
-        <v>18</v>
-      </c>
-      <c r="D76">
+      <c r="C76" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C77" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77">
+      <c r="C77" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C78" t="s">
-        <v>18</v>
-      </c>
-      <c r="D78">
+      <c r="C78" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C79" t="s">
-        <v>18</v>
-      </c>
-      <c r="D79">
+      <c r="C79" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D79" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C80" t="s">
-        <v>18</v>
-      </c>
-      <c r="D80">
+      <c r="C80" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D81">
+      <c r="C81" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C82" t="s">
-        <v>18</v>
-      </c>
-      <c r="D82">
+      <c r="C82" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C83" t="s">
-        <v>18</v>
-      </c>
-      <c r="D83">
+      <c r="C83" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D83" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C84" t="s">
-        <v>18</v>
-      </c>
-      <c r="D84">
+      <c r="C84" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" s="2">
         <v>1206</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="1">
         <v>402</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B104" t="s">
-        <v>151</v>
-      </c>
-      <c r="C104">
-        <v>1206</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="B104" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C104" s="1">
+        <v>1206</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C105" t="s">
-        <v>151</v>
-      </c>
-      <c r="D105">
+      <c r="C105" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D105" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="A106" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C106" t="s">
-        <v>151</v>
-      </c>
-      <c r="D106">
+      <c r="C106" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D106" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C107" t="s">
-        <v>151</v>
-      </c>
-      <c r="D107">
+      <c r="C107" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D107" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C108" t="s">
-        <v>151</v>
-      </c>
-      <c r="D108">
+      <c r="C108" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D108" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C109" t="s">
-        <v>151</v>
-      </c>
-      <c r="D109">
+      <c r="C109" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D109" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C110" t="s">
-        <v>151</v>
-      </c>
-      <c r="D110">
+      <c r="C110" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D110" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C111" t="s">
-        <v>151</v>
-      </c>
-      <c r="D111">
+      <c r="C111" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D111" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C112" t="s">
-        <v>151</v>
-      </c>
-      <c r="D112">
+      <c r="C112" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D112" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="1">
         <v>51</v>
       </c>
-      <c r="C113" t="s">
-        <v>151</v>
-      </c>
-      <c r="D113">
+      <c r="C113" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D113" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="1">
         <v>51</v>
       </c>
-      <c r="C114" t="s">
-        <v>151</v>
-      </c>
-      <c r="D114">
+      <c r="C114" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D114" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="1">
         <v>51</v>
       </c>
-      <c r="C115" t="s">
-        <v>151</v>
-      </c>
-      <c r="D115">
+      <c r="C115" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D115" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="1">
         <v>51</v>
       </c>
-      <c r="C116" t="s">
-        <v>151</v>
-      </c>
-      <c r="D116">
+      <c r="C116" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D116" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="1">
         <v>200</v>
       </c>
-      <c r="C117" t="s">
-        <v>151</v>
-      </c>
-      <c r="D117">
+      <c r="C117" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D117" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="1">
         <v>200</v>
       </c>
-      <c r="C118" t="s">
-        <v>151</v>
-      </c>
-      <c r="D118">
+      <c r="C118" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D118" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C119" t="s">
-        <v>151</v>
-      </c>
-      <c r="D119">
+      <c r="C119" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D119" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C120" t="s">
-        <v>151</v>
-      </c>
-      <c r="D120">
+      <c r="C120" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D120" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C121" t="s">
-        <v>151</v>
-      </c>
-      <c r="D121">
+      <c r="C121" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D121" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="1">
         <v>330</v>
       </c>
-      <c r="C122" t="s">
-        <v>151</v>
-      </c>
-      <c r="D122">
+      <c r="C122" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D122" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="1">
         <v>330</v>
       </c>
-      <c r="C123" t="s">
-        <v>151</v>
-      </c>
-      <c r="D123">
+      <c r="C123" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D123" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="A124" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C124" t="s">
-        <v>151</v>
-      </c>
-      <c r="D124">
+      <c r="C124" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D124" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C125" t="s">
-        <v>151</v>
-      </c>
-      <c r="D125">
+      <c r="C125" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D125" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="A126" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C126" t="s">
-        <v>151</v>
-      </c>
-      <c r="D126">
+      <c r="C126" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D126" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="A127" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C127" t="s">
-        <v>151</v>
-      </c>
-      <c r="D127">
+      <c r="C127" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D127" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="A128" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C128" t="s">
-        <v>151</v>
-      </c>
-      <c r="D128">
+      <c r="C128" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D128" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C129" t="s">
-        <v>151</v>
-      </c>
-      <c r="D129">
+      <c r="C129" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D129" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="A130" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="1">
         <v>120</v>
       </c>
-      <c r="C130" t="s">
-        <v>151</v>
-      </c>
-      <c r="D130">
+      <c r="C130" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D130" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="1">
         <v>120</v>
       </c>
-      <c r="C131" t="s">
-        <v>151</v>
-      </c>
-      <c r="D131">
+      <c r="C131" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D131" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="1">
         <v>120</v>
       </c>
-      <c r="C132" t="s">
-        <v>151</v>
-      </c>
-      <c r="D132">
+      <c r="C132" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D132" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="1">
         <v>120</v>
       </c>
-      <c r="C133" t="s">
-        <v>151</v>
-      </c>
-      <c r="D133">
+      <c r="C133" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D133" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="1">
         <v>120</v>
       </c>
-      <c r="C134" t="s">
-        <v>151</v>
-      </c>
-      <c r="D134">
+      <c r="C134" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D134" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="1">
         <v>120</v>
       </c>
-      <c r="C135" t="s">
-        <v>151</v>
-      </c>
-      <c r="D135">
+      <c r="C135" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D135" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="A136" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="1">
         <v>120</v>
       </c>
-      <c r="C136" t="s">
-        <v>151</v>
-      </c>
-      <c r="D136">
+      <c r="C136" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D136" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A137" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="1">
         <v>120</v>
       </c>
-      <c r="C137" t="s">
-        <v>151</v>
-      </c>
-      <c r="D137">
+      <c r="C137" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D137" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="A138" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="1">
         <v>120</v>
       </c>
-      <c r="C138" t="s">
-        <v>151</v>
-      </c>
-      <c r="D138">
+      <c r="C138" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D138" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="A139" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="1">
         <v>120</v>
       </c>
-      <c r="C139" t="s">
-        <v>151</v>
-      </c>
-      <c r="D139">
+      <c r="C139" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D139" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="A140" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="1">
         <v>120</v>
       </c>
-      <c r="C140" t="s">
-        <v>151</v>
-      </c>
-      <c r="D140">
+      <c r="C140" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D140" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="A141" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="1">
         <v>120</v>
       </c>
-      <c r="C141" t="s">
-        <v>151</v>
-      </c>
-      <c r="D141">
+      <c r="C141" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D141" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="A142" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="1">
         <v>120</v>
       </c>
-      <c r="C142" t="s">
-        <v>151</v>
-      </c>
-      <c r="D142">
+      <c r="C142" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D142" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="A143" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="1">
         <v>120</v>
       </c>
-      <c r="C143" t="s">
-        <v>151</v>
-      </c>
-      <c r="D143">
+      <c r="C143" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D143" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="A144" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="1">
         <v>120</v>
       </c>
-      <c r="C144" t="s">
-        <v>151</v>
-      </c>
-      <c r="D144">
+      <c r="C144" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D144" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="A145" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="1">
         <v>120</v>
       </c>
-      <c r="C145" t="s">
-        <v>151</v>
-      </c>
-      <c r="D145">
+      <c r="C145" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D145" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="A146" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="1">
         <v>120</v>
       </c>
-      <c r="C146" t="s">
-        <v>151</v>
-      </c>
-      <c r="D146">
+      <c r="C146" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D146" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="A147" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="1">
         <v>120</v>
       </c>
-      <c r="C147" t="s">
-        <v>151</v>
-      </c>
-      <c r="D147">
+      <c r="C147" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D147" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="A148" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="1">
         <v>120</v>
       </c>
-      <c r="C148" t="s">
-        <v>151</v>
-      </c>
-      <c r="D148">
+      <c r="C148" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D148" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="A149" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="1">
         <v>120</v>
       </c>
-      <c r="C149" t="s">
-        <v>151</v>
-      </c>
-      <c r="D149">
+      <c r="C149" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D149" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="A150" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="1">
         <v>120</v>
       </c>
-      <c r="C150" t="s">
-        <v>151</v>
-      </c>
-      <c r="D150">
+      <c r="C150" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D150" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="A151" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="1">
         <v>120</v>
       </c>
-      <c r="C151" t="s">
-        <v>151</v>
-      </c>
-      <c r="D151">
+      <c r="C151" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D151" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="A152" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="1">
         <v>120</v>
       </c>
-      <c r="C152" t="s">
-        <v>151</v>
-      </c>
-      <c r="D152">
+      <c r="C152" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D152" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="A153" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="1">
         <v>120</v>
       </c>
-      <c r="C153" t="s">
-        <v>151</v>
-      </c>
-      <c r="D153">
+      <c r="C153" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D153" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="A154" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="1">
         <v>120</v>
       </c>
-      <c r="C154" t="s">
-        <v>151</v>
-      </c>
-      <c r="D154">
+      <c r="C154" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D154" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="A155" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B155">
+      <c r="B155" s="1">
         <v>120</v>
       </c>
-      <c r="C155" t="s">
-        <v>151</v>
-      </c>
-      <c r="D155">
+      <c r="C155" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D155" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="A156" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B156">
+      <c r="B156" s="1">
         <v>120</v>
       </c>
-      <c r="C156" t="s">
-        <v>151</v>
-      </c>
-      <c r="D156">
+      <c r="C156" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D156" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="A157" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B157">
+      <c r="B157" s="1">
         <v>120</v>
       </c>
-      <c r="C157" t="s">
-        <v>151</v>
-      </c>
-      <c r="D157">
+      <c r="C157" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D157" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="A158" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B158">
+      <c r="B158" s="1">
         <v>120</v>
       </c>
-      <c r="C158" t="s">
-        <v>151</v>
-      </c>
-      <c r="D158">
+      <c r="C158" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D158" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="A159" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B159">
+      <c r="B159" s="1">
         <v>120</v>
       </c>
-      <c r="C159" t="s">
-        <v>151</v>
-      </c>
-      <c r="D159">
+      <c r="C159" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D159" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="A160" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="1">
         <v>120</v>
       </c>
-      <c r="C160" t="s">
-        <v>151</v>
-      </c>
-      <c r="D160">
+      <c r="C160" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D160" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="A161" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="1">
         <v>120</v>
       </c>
-      <c r="C161" t="s">
-        <v>151</v>
-      </c>
-      <c r="D161">
+      <c r="C161" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D161" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="A162" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B162">
+      <c r="B162" s="1">
         <v>120</v>
       </c>
-      <c r="C162" t="s">
-        <v>151</v>
-      </c>
-      <c r="D162">
+      <c r="C162" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D162" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="A163" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="1">
         <v>120</v>
       </c>
-      <c r="C163" t="s">
-        <v>151</v>
-      </c>
-      <c r="D163">
+      <c r="C163" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D163" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="A164" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B164">
+      <c r="B164" s="1">
         <v>120</v>
       </c>
-      <c r="C164" t="s">
-        <v>151</v>
-      </c>
-      <c r="D164">
+      <c r="C164" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D164" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="A165" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B165">
+      <c r="B165" s="1">
         <v>120</v>
       </c>
-      <c r="C165" t="s">
-        <v>151</v>
-      </c>
-      <c r="D165">
+      <c r="C165" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D165" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="A166" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B166">
+      <c r="B166" s="1">
         <v>120</v>
       </c>
-      <c r="C166" t="s">
-        <v>151</v>
-      </c>
-      <c r="D166">
+      <c r="C166" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D166" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="A167" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B167">
+      <c r="B167" s="1">
         <v>120</v>
       </c>
-      <c r="C167" t="s">
-        <v>151</v>
-      </c>
-      <c r="D167">
+      <c r="C167" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D167" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="A168" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B168">
+      <c r="B168" s="1">
         <v>120</v>
       </c>
-      <c r="C168" t="s">
-        <v>151</v>
-      </c>
-      <c r="D168">
+      <c r="C168" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D168" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="A169" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B169">
+      <c r="B169" s="1">
         <v>120</v>
       </c>
-      <c r="C169" t="s">
-        <v>151</v>
-      </c>
-      <c r="D169">
+      <c r="C169" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D169" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="A170" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C170" t="s">
-        <v>151</v>
-      </c>
-      <c r="D170">
+      <c r="C170" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D170" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="A171" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C171" t="s">
-        <v>151</v>
-      </c>
-      <c r="D171">
+      <c r="C171" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D171" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="A172" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C172" t="s">
-        <v>151</v>
-      </c>
-      <c r="D172">
+      <c r="C172" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D172" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="A173" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B173">
+      <c r="B173" s="1">
         <v>330</v>
       </c>
-      <c r="C173" t="s">
-        <v>151</v>
-      </c>
-      <c r="D173">
+      <c r="C173" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D173" s="1">
         <v>1206</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="A174" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B174" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="A175" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="A176" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C176" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="A177" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+      <c r="A178" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+      <c r="A179" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+      <c r="A180" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+      <c r="A181" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="A182" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="A183" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="A184" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="A185" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="A186" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C186" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="A187" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="A188" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="A189" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="A190" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C190" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="A191" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="A192" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C192" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="A193" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C193" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="A194" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C194" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="A195" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="A196" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="A197" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C197" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+      <c r="A198" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C198" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="A199" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+      <c r="A200" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C200" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+      <c r="A201" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B201" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C201" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D201" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+      <c r="A202" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C202" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D202" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+      <c r="A203" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B203" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C203" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D203" s="1" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+      <c r="A204" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C204" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D204" t="s">
+      <c r="D204" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+      <c r="A205" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C205" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D205" t="s">
+      <c r="D205" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+      <c r="A206" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C206" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D206" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+      <c r="A207" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B207" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C207" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D207" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+      <c r="A208" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="A209" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B209" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C209" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+      <c r="A210" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C210" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+      <c r="A211" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C211" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="1" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+      <c r="A212" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C212" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D212">
+      <c r="D212" s="1">
         <v>60050685100</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+      <c r="A213" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C213" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D213" s="1" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+      <c r="A214" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C214" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D214" s="1" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="A215" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B215" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C215" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="1" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="A216" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B216" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="1" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="A217" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="1" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+      <c r="A218" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C218" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D218" s="1" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+      <c r="A219" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B219" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="1" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+      <c r="A220" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B220" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C220" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D220" t="s">
+      <c r="D220" s="1" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+      <c r="A221" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B221" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C221" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D221" s="1" t="s">
         <v>288</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D221"/>
+  <hyperlinks>
+    <hyperlink ref="I5" r:id="rId1"/>
+    <hyperlink ref="I6" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I7" r:id="rId4"/>
+    <hyperlink ref="I3" r:id="rId5"/>
+    <hyperlink ref="I2" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+    <hyperlink ref="I9" r:id="rId8"/>
+    <hyperlink ref="I10" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>